<commit_message>
stationdata 엑셀 파일 수정
</commit_message>
<xml_diff>
--- a/app/src/main/assets/stationdata_new.xlsx
+++ b/app/src/main/assets/stationdata_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HyukSu\Desktop\git_new\SubwayAlarm-android-app\app\src\main\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CC16B4-85A4-4AD7-B630-28A08824969E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77554315-AC95-4329-84D5-940FA2781AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="14400" windowHeight="7460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="역정보" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="619">
   <si>
     <t>건대입구</t>
   </si>
@@ -1255,501 +1255,491 @@
     <t>미금</t>
   </si>
   <si>
+    <t>오산대</t>
+  </si>
+  <si>
+    <t>진위</t>
+  </si>
+  <si>
+    <t>가능</t>
+  </si>
+  <si>
+    <t>증산(명지대앞)</t>
+  </si>
+  <si>
+    <t>면목</t>
+  </si>
+  <si>
+    <t>사가정</t>
+  </si>
+  <si>
+    <t>신풍</t>
+  </si>
+  <si>
+    <t>남구로</t>
+  </si>
+  <si>
+    <t>주엽</t>
+  </si>
+  <si>
+    <t>산본</t>
+  </si>
+  <si>
+    <t>한대앞</t>
+  </si>
+  <si>
+    <t>안국</t>
+  </si>
+  <si>
+    <t>수진</t>
+  </si>
+  <si>
+    <t>구반포</t>
+  </si>
+  <si>
+    <t>소래포구</t>
+  </si>
+  <si>
+    <t>구룡</t>
+  </si>
+  <si>
+    <t>신갈</t>
+  </si>
+  <si>
+    <t>송내</t>
+  </si>
+  <si>
+    <t>망월사</t>
+  </si>
+  <si>
+    <t>도봉</t>
+  </si>
+  <si>
+    <t>외대앞</t>
+  </si>
+  <si>
+    <t>신이문</t>
+  </si>
+  <si>
+    <t>아산</t>
+  </si>
+  <si>
+    <t>배방</t>
+  </si>
+  <si>
+    <t>온양온천</t>
+  </si>
+  <si>
+    <t>고덕</t>
+  </si>
+  <si>
+    <t>독바위</t>
+  </si>
+  <si>
+    <t>새절(신사)</t>
+  </si>
+  <si>
+    <t>상수</t>
+  </si>
+  <si>
+    <t>보문</t>
+  </si>
+  <si>
+    <t>상월곡(한국과학기술연구원)</t>
+  </si>
+  <si>
+    <t>화랑대(서울여대입구)</t>
+  </si>
+  <si>
+    <t>중화</t>
+  </si>
+  <si>
+    <t>봉은사</t>
+  </si>
+  <si>
+    <t>서대문</t>
+  </si>
+  <si>
+    <t>원인재</t>
+  </si>
+  <si>
+    <t>대모산</t>
+  </si>
+  <si>
+    <t>구성</t>
+  </si>
+  <si>
+    <t>독산</t>
+  </si>
+  <si>
+    <t>원덕</t>
+  </si>
+  <si>
+    <t>동두천</t>
+  </si>
+  <si>
+    <t>회룡</t>
+  </si>
+  <si>
+    <t>봉명</t>
+  </si>
+  <si>
+    <t>안암(고대병원앞)</t>
+  </si>
+  <si>
+    <t>인천공항2터미널</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마곡나루</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>청량리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>초지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>고잔</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>중앙</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>한대앞</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>야목</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>어천</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>오목천</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>고색</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>강일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>미사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>하남풍산</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>하남시청</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>하남검단산</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>탕정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>양재</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>양재시민의숲</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>청계산입구</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>판교</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>정자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>동천</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>수지구청</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>성복</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상현</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>광교중앙</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>광교</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>산곡</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>석남</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼전</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>석촌고분</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>석촌</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>송파나루</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>한성백제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>둔촌오륜</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>중앙보훈병원</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>올림픽공원</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지평</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>청라국제도시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>영종</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인천공항1터미널</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>청량리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>회기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>중랑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>광운대</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인하대</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>숭의</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>신포</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인천</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>안산</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>신길온천</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>정왕</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>미금</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>용유</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>워터파크</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>합동청사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>장기주차장</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인천공항1터미널</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파라다이스 시티</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>보문</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>솔밭공원</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>가오리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>화계</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼양</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼양사거리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>솔샘</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>북한산보국문</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>정릉</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>성신여대입구</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.19 민주묘지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>잠실새내</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>남위례</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>여의도</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>신내</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>역촌</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>공덕</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>신논현</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>논현</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>신사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>신답</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>까치산</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>신정네거리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>양천구청</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>도림천</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>응암순환(상선)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>구산</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>기흥</t>
-  </si>
-  <si>
-    <t>오산대</t>
-  </si>
-  <si>
-    <t>진위</t>
-  </si>
-  <si>
-    <t>가능</t>
-  </si>
-  <si>
-    <t>증산(명지대앞)</t>
-  </si>
-  <si>
-    <t>면목</t>
-  </si>
-  <si>
-    <t>사가정</t>
-  </si>
-  <si>
-    <t>신풍</t>
-  </si>
-  <si>
-    <t>남구로</t>
-  </si>
-  <si>
-    <t>주엽</t>
-  </si>
-  <si>
-    <t>산본</t>
-  </si>
-  <si>
-    <t>한대앞</t>
-  </si>
-  <si>
-    <t>안국</t>
-  </si>
-  <si>
-    <t>수진</t>
-  </si>
-  <si>
-    <t>구반포</t>
-  </si>
-  <si>
-    <t>소래포구</t>
-  </si>
-  <si>
-    <t>구룡</t>
-  </si>
-  <si>
-    <t>신갈</t>
-  </si>
-  <si>
-    <t>송내</t>
-  </si>
-  <si>
-    <t>망월사</t>
-  </si>
-  <si>
-    <t>도봉</t>
-  </si>
-  <si>
-    <t>외대앞</t>
-  </si>
-  <si>
-    <t>신이문</t>
-  </si>
-  <si>
-    <t>아산</t>
-  </si>
-  <si>
-    <t>배방</t>
-  </si>
-  <si>
-    <t>온양온천</t>
-  </si>
-  <si>
-    <t>고덕</t>
-  </si>
-  <si>
-    <t>독바위</t>
-  </si>
-  <si>
-    <t>새절(신사)</t>
-  </si>
-  <si>
-    <t>상수</t>
-  </si>
-  <si>
-    <t>보문</t>
-  </si>
-  <si>
-    <t>상월곡(한국과학기술연구원)</t>
-  </si>
-  <si>
-    <t>화랑대(서울여대입구)</t>
-  </si>
-  <si>
-    <t>중화</t>
-  </si>
-  <si>
-    <t>봉은사</t>
-  </si>
-  <si>
-    <t>서대문</t>
-  </si>
-  <si>
-    <t>원인재</t>
-  </si>
-  <si>
-    <t>대모산</t>
-  </si>
-  <si>
-    <t>구성</t>
-  </si>
-  <si>
-    <t>독산</t>
-  </si>
-  <si>
-    <t>원덕</t>
-  </si>
-  <si>
-    <t>동두천</t>
-  </si>
-  <si>
-    <t>회룡</t>
-  </si>
-  <si>
-    <t>봉명</t>
-  </si>
-  <si>
-    <t>쌍용(나사렛대)</t>
-  </si>
-  <si>
-    <t>안암(고대병원앞)</t>
-  </si>
-  <si>
-    <t>인천공항2터미널</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>마곡나루</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>청량리</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>초지</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>고잔</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>중앙</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>한대앞</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>사리</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>야목</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>어천</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>오목천</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>고색</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>강일</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>미사</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>하남풍산</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>하남시청</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>하남검단산</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>탕정</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>양재</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>양재시민의숲</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>청계산입구</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>판교</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>정자</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>동천</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>수지구청</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>성복</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>상현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>광교중앙</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>광교</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>산곡</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>석남</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>삼전</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>석촌고분</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>석촌</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>송파나루</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>한성백제</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>둔촌오륜</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>중앙보훈병원</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>올림픽공원</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>지평</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>청라국제도시</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>영종</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>인천공항1터미널</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>청량리</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>회기</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>중랑</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>광운대</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>인하대</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>숭의</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>신포</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>인천</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>안산</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>신길온천</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>정왕</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>미금</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>용유</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>워터파크</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>합동청사</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>장기주차장</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>인천공항1터미널</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>파라다이스 시티</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>보문</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>북산한우이</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>솔밭공원</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>가오리</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>화계</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>삼양</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>삼양사거리</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>솔샘</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>북한산보국문</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>정릉</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>성신여대입구</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.19 민주묘지</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>잠실새내</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>남위례</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>여의도</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>신내</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>역촌</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>공덕</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>신논현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>논현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>신사</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>신답</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>까치산</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>신정네거리</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>양천구청</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>도림천</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>응암순환(상선)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>구산</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>기흥</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -2028,10 +2018,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>10,13</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>10,12</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -2041,6 +2027,18 @@
   </si>
   <si>
     <t>13,14</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>북한산우이</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>쌍용</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>강매</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2437,8 +2435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C636"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A571" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D579" sqref="D579"/>
+    <sheetView tabSelected="1" topLeftCell="A484" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C461" sqref="C461"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -2467,7 +2465,7 @@
         <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2555,7 +2553,7 @@
         <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2577,7 +2575,7 @@
         <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2588,12 +2586,12 @@
         <v>112</v>
       </c>
       <c r="C13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="6" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B14" s="3">
         <v>113</v>
@@ -2610,7 +2608,7 @@
         <v>114</v>
       </c>
       <c r="C15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2626,7 +2624,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="6" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B17" s="3">
         <v>116</v>
@@ -2659,7 +2657,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="6" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B20" s="3">
         <v>119</v>
@@ -2670,7 +2668,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="6" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B21" s="3">
         <v>120</v>
@@ -2687,7 +2685,7 @@
         <v>121</v>
       </c>
       <c r="C22" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2698,12 +2696,12 @@
         <v>122</v>
       </c>
       <c r="C23" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="6" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B24" s="3">
         <v>123</v>
@@ -2714,7 +2712,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B25" s="3">
         <v>124</v>
@@ -2736,7 +2734,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="6" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B27" s="3">
         <v>126</v>
@@ -2747,7 +2745,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="6" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B28" s="3">
         <v>127</v>
@@ -2758,7 +2756,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="6" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B29" s="3">
         <v>128</v>
@@ -2780,7 +2778,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="6" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B31" s="3">
         <v>130</v>
@@ -2802,7 +2800,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="6" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B33" s="3">
         <v>132</v>
@@ -2813,7 +2811,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="6" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B34" s="3">
         <v>133</v>
@@ -2835,7 +2833,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="6" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B36" s="3">
         <v>135</v>
@@ -2846,7 +2844,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B37" s="3">
         <v>136</v>
@@ -2868,7 +2866,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B39" s="3">
         <v>138</v>
@@ -2890,7 +2888,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="6" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B41" s="3">
         <v>140</v>
@@ -2907,7 +2905,7 @@
         <v>141</v>
       </c>
       <c r="C42" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2945,7 +2943,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="6" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B46" s="3">
         <v>145</v>
@@ -3006,7 +3004,7 @@
         <v>150</v>
       </c>
       <c r="C51" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -3099,7 +3097,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B60" s="3">
         <v>159</v>
@@ -3121,18 +3119,18 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="6" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B62" s="3">
         <v>161</v>
       </c>
       <c r="C62" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="6" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B63" s="3">
         <v>162</v>
@@ -3149,7 +3147,7 @@
         <v>163</v>
       </c>
       <c r="C64" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -3209,7 +3207,7 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="6" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B70" s="3">
         <v>169</v>
@@ -3220,7 +3218,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B71" s="3">
         <v>170</v>
@@ -3264,7 +3262,7 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B75" s="3">
         <v>174</v>
@@ -3275,7 +3273,7 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="6" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B76" s="3">
         <v>175</v>
@@ -3319,13 +3317,13 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B80" s="3">
         <v>179</v>
       </c>
       <c r="C80" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -3347,7 +3345,7 @@
         <v>181</v>
       </c>
       <c r="C82" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -3396,7 +3394,7 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B87" s="3">
         <v>186</v>
@@ -3440,13 +3438,13 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B91" s="3">
         <v>190</v>
       </c>
       <c r="C91" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -3457,7 +3455,7 @@
         <v>191</v>
       </c>
       <c r="C92" t="s">
-        <v>455</v>
+        <v>617</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -3468,18 +3466,18 @@
         <v>192</v>
       </c>
       <c r="C93" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B94" s="3">
         <v>193</v>
       </c>
       <c r="C94" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -3490,7 +3488,7 @@
         <v>194</v>
       </c>
       <c r="C95" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -3501,7 +3499,7 @@
         <v>195</v>
       </c>
       <c r="C96" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -3512,12 +3510,12 @@
         <v>196</v>
       </c>
       <c r="C97" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="6" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B98" s="3">
         <v>200</v>
@@ -3528,7 +3526,7 @@
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="6" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B99" s="3">
         <v>201</v>
@@ -3539,7 +3537,7 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B100" s="3">
         <v>202</v>
@@ -3572,7 +3570,7 @@
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="6" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B103" s="3">
         <v>205</v>
@@ -3583,7 +3581,7 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" s="6" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B104" s="3">
         <v>206</v>
@@ -3594,7 +3592,7 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="6" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B105" s="3">
         <v>207</v>
@@ -3605,7 +3603,7 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="6" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B106" s="3">
         <v>208</v>
@@ -3627,18 +3625,18 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="6" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B108" s="3">
         <v>210</v>
       </c>
       <c r="C108" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="6" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B109" s="3">
         <v>211</v>
@@ -3649,7 +3647,7 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B110" s="3">
         <v>212</v>
@@ -3693,7 +3691,7 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B114" s="3">
         <v>216</v>
@@ -3715,7 +3713,7 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="6" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="B116" s="3">
         <v>218</v>
@@ -3748,7 +3746,7 @@
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="6" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B119" s="3">
         <v>221</v>
@@ -3759,7 +3757,7 @@
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="6" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B120" s="3">
         <v>222</v>
@@ -3781,7 +3779,7 @@
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="6" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B122" s="3">
         <v>224</v>
@@ -3803,7 +3801,7 @@
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="6" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B124" s="3">
         <v>226</v>
@@ -3820,12 +3818,12 @@
         <v>227</v>
       </c>
       <c r="C125" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="6" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B126" s="3">
         <v>228</v>
@@ -3869,7 +3867,7 @@
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="6" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B130" s="3">
         <v>232</v>
@@ -3886,7 +3884,7 @@
         <v>233</v>
       </c>
       <c r="C131" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -3902,7 +3900,7 @@
     </row>
     <row r="133" spans="1:3">
       <c r="A133" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B133" s="3">
         <v>235</v>
@@ -3913,7 +3911,7 @@
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="6" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B134" s="3">
         <v>236</v>
@@ -3935,7 +3933,7 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="6" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B136" s="3">
         <v>238</v>
@@ -3946,7 +3944,7 @@
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="6" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B137" s="3">
         <v>239</v>
@@ -3957,7 +3955,7 @@
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="6" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B138" s="3">
         <v>240</v>
@@ -3968,7 +3966,7 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="6" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B139" s="3">
         <v>241</v>
@@ -3996,7 +3994,7 @@
         <v>243</v>
       </c>
       <c r="C141" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -4007,7 +4005,7 @@
         <v>244</v>
       </c>
       <c r="C142" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -4023,7 +4021,7 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="6" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B144" s="3">
         <v>246</v>
@@ -4034,13 +4032,13 @@
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="6" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B145" s="3">
         <v>247</v>
       </c>
       <c r="C145" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -4051,7 +4049,7 @@
         <v>248</v>
       </c>
       <c r="C146" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -4062,7 +4060,7 @@
         <v>249</v>
       </c>
       <c r="C147" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -4073,7 +4071,7 @@
         <v>250</v>
       </c>
       <c r="C148" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -4089,13 +4087,13 @@
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B150" s="3">
         <v>301</v>
       </c>
       <c r="C150" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -4133,7 +4131,7 @@
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="6" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B154" s="3">
         <v>305</v>
@@ -4177,7 +4175,7 @@
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B158" s="3">
         <v>309</v>
@@ -4210,7 +4208,7 @@
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="6" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B161" s="3">
         <v>312</v>
@@ -4221,7 +4219,7 @@
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="6" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B162" s="3">
         <v>313</v>
@@ -4232,7 +4230,7 @@
     </row>
     <row r="163" spans="1:3">
       <c r="A163" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B163" s="3">
         <v>314</v>
@@ -4265,7 +4263,7 @@
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B166" s="3">
         <v>317</v>
@@ -4293,12 +4291,12 @@
         <v>319</v>
       </c>
       <c r="C168" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="6" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B169" s="3">
         <v>320</v>
@@ -4309,7 +4307,7 @@
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="6" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B170" s="3">
         <v>321</v>
@@ -4320,7 +4318,7 @@
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="6" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B171" s="3">
         <v>322</v>
@@ -4342,7 +4340,7 @@
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="6" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B173" s="3">
         <v>324</v>
@@ -4364,7 +4362,7 @@
     </row>
     <row r="175" spans="1:3">
       <c r="A175" s="6" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B175" s="3">
         <v>326</v>
@@ -4386,7 +4384,7 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="6" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B177" s="3">
         <v>328</v>
@@ -4408,7 +4406,7 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179" s="6" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B179" s="3">
         <v>330</v>
@@ -4419,7 +4417,7 @@
     </row>
     <row r="180" spans="1:3">
       <c r="A180" s="6" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B180" s="3">
         <v>331</v>
@@ -4441,7 +4439,7 @@
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="6" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B182" s="3">
         <v>333</v>
@@ -4452,7 +4450,7 @@
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B183" s="3">
         <v>334</v>
@@ -4463,7 +4461,7 @@
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="6" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B184" s="3">
         <v>335</v>
@@ -4507,7 +4505,7 @@
     </row>
     <row r="188" spans="1:3">
       <c r="A188" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B188" s="3">
         <v>339</v>
@@ -4518,7 +4516,7 @@
     </row>
     <row r="189" spans="1:3">
       <c r="A189" s="6" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B189" s="3">
         <v>340</v>
@@ -4529,7 +4527,7 @@
     </row>
     <row r="190" spans="1:3">
       <c r="A190" s="6" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="B190" s="3">
         <v>341</v>
@@ -4551,7 +4549,7 @@
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="6" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B192" s="3">
         <v>343</v>
@@ -4562,7 +4560,7 @@
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B193" s="3">
         <v>400</v>
@@ -4573,7 +4571,7 @@
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B194" s="3">
         <v>401</v>
@@ -4584,7 +4582,7 @@
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B195" s="3">
         <v>402</v>
@@ -4595,7 +4593,7 @@
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B196" s="3">
         <v>403</v>
@@ -4606,7 +4604,7 @@
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="6" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B197" s="3">
         <v>404</v>
@@ -4617,7 +4615,7 @@
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B198" s="3">
         <v>405</v>
@@ -4628,7 +4626,7 @@
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B199" s="3">
         <v>406</v>
@@ -4639,13 +4637,13 @@
     </row>
     <row r="200" spans="1:3">
       <c r="A200" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B200" s="3">
         <v>407</v>
       </c>
       <c r="C200" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -4694,18 +4692,18 @@
     </row>
     <row r="205" spans="1:3">
       <c r="A205" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B205" s="3">
         <v>412</v>
       </c>
       <c r="C205" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" s="6" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B206" s="3">
         <v>413</v>
@@ -4771,7 +4769,7 @@
     </row>
     <row r="212" spans="1:3">
       <c r="A212" s="6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B212" s="3">
         <v>419</v>
@@ -4815,7 +4813,7 @@
     </row>
     <row r="216" spans="1:3">
       <c r="A216" s="6" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="B216" s="3">
         <v>423</v>
@@ -4826,7 +4824,7 @@
     </row>
     <row r="217" spans="1:3">
       <c r="A217" s="6" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B217" s="3">
         <v>424</v>
@@ -4837,7 +4835,7 @@
     </row>
     <row r="218" spans="1:3">
       <c r="A218" s="6" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B218" s="3">
         <v>425</v>
@@ -4848,7 +4846,7 @@
     </row>
     <row r="219" spans="1:3">
       <c r="A219" s="6" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B219" s="3">
         <v>426</v>
@@ -4870,7 +4868,7 @@
     </row>
     <row r="221" spans="1:3">
       <c r="A221" s="6" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="B221" s="3">
         <v>428</v>
@@ -4892,7 +4890,7 @@
     </row>
     <row r="223" spans="1:3">
       <c r="A223" s="6" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B223" s="3">
         <v>430</v>
@@ -4925,7 +4923,7 @@
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="6" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B226" s="3">
         <v>433</v>
@@ -4936,7 +4934,7 @@
     </row>
     <row r="227" spans="1:3">
       <c r="A227" s="6" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B227" s="3">
         <v>434</v>
@@ -4947,7 +4945,7 @@
     </row>
     <row r="228" spans="1:3">
       <c r="A228" s="6" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B228" s="3">
         <v>435</v>
@@ -4980,7 +4978,7 @@
     </row>
     <row r="231" spans="1:3">
       <c r="A231" s="6" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="B231" s="3">
         <v>438</v>
@@ -5002,7 +5000,7 @@
     </row>
     <row r="233" spans="1:3">
       <c r="A233" s="6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B233" s="3">
         <v>440</v>
@@ -5046,7 +5044,7 @@
     </row>
     <row r="237" spans="1:3">
       <c r="A237" s="6" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B237" s="3">
         <v>444</v>
@@ -5057,7 +5055,7 @@
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="6" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B238" s="3">
         <v>445</v>
@@ -5090,7 +5088,7 @@
     </row>
     <row r="241" spans="1:3">
       <c r="A241" s="6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B241" s="3">
         <v>500</v>
@@ -5112,7 +5110,7 @@
     </row>
     <row r="243" spans="1:3">
       <c r="A243" s="6" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B243" s="3">
         <v>502</v>
@@ -5145,7 +5143,7 @@
     </row>
     <row r="246" spans="1:3">
       <c r="A246" s="6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B246" s="3">
         <v>505</v>
@@ -5178,7 +5176,7 @@
     </row>
     <row r="249" spans="1:3">
       <c r="A249" s="6" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B249" s="3">
         <v>508</v>
@@ -5222,7 +5220,7 @@
     </row>
     <row r="253" spans="1:3">
       <c r="A253" s="6" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="B253" s="3">
         <v>512</v>
@@ -5233,7 +5231,7 @@
     </row>
     <row r="254" spans="1:3">
       <c r="A254" s="6" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B254" s="3">
         <v>513</v>
@@ -5255,7 +5253,7 @@
     </row>
     <row r="256" spans="1:3">
       <c r="A256" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B256" s="3">
         <v>515</v>
@@ -5266,13 +5264,13 @@
     </row>
     <row r="257" spans="1:3">
       <c r="A257" s="6" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="B257" s="3">
         <v>516</v>
       </c>
       <c r="C257" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -5299,7 +5297,7 @@
     </row>
     <row r="260" spans="1:3">
       <c r="A260" s="6" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="B260" s="3">
         <v>519</v>
@@ -5321,7 +5319,7 @@
     </row>
     <row r="262" spans="1:3">
       <c r="A262" s="6" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B262" s="3">
         <v>521</v>
@@ -5338,7 +5336,7 @@
         <v>522</v>
       </c>
       <c r="C263" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -5354,7 +5352,7 @@
     </row>
     <row r="265" spans="1:3">
       <c r="A265" s="6" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B265" s="3">
         <v>524</v>
@@ -5365,7 +5363,7 @@
     </row>
     <row r="266" spans="1:3">
       <c r="A266" s="6" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B266" s="3">
         <v>525</v>
@@ -5376,7 +5374,7 @@
     </row>
     <row r="267" spans="1:3">
       <c r="A267" s="6" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B267" s="3">
         <v>526</v>
@@ -5387,7 +5385,7 @@
     </row>
     <row r="268" spans="1:3">
       <c r="A268" s="6" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="B268" s="3">
         <v>527</v>
@@ -5398,7 +5396,7 @@
     </row>
     <row r="269" spans="1:3">
       <c r="A269" s="6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B269" s="3">
         <v>528</v>
@@ -5420,7 +5418,7 @@
     </row>
     <row r="271" spans="1:3">
       <c r="A271" s="6" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B271" s="3">
         <v>530</v>
@@ -5464,7 +5462,7 @@
     </row>
     <row r="275" spans="1:3">
       <c r="A275" s="6" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="B275" s="3">
         <v>534</v>
@@ -5497,7 +5495,7 @@
     </row>
     <row r="278" spans="1:3">
       <c r="A278" s="6" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="B278" s="3">
         <v>537</v>
@@ -5514,7 +5512,7 @@
         <v>538</v>
       </c>
       <c r="C279" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="280" spans="1:3">
@@ -5552,7 +5550,7 @@
     </row>
     <row r="283" spans="1:3">
       <c r="A283" s="6" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B283" s="3">
         <v>542</v>
@@ -5591,7 +5589,7 @@
         <v>545</v>
       </c>
       <c r="C286" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="287" spans="1:3">
@@ -5629,13 +5627,13 @@
     </row>
     <row r="290" spans="1:3">
       <c r="A290" s="6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B290" s="3">
         <v>549</v>
       </c>
       <c r="C290" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="291" spans="1:3">
@@ -5657,7 +5655,7 @@
         <v>551</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="293" spans="1:3">
@@ -5668,7 +5666,7 @@
         <v>552</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="294" spans="1:3">
@@ -5679,7 +5677,7 @@
         <v>553</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="295" spans="1:3">
@@ -5690,7 +5688,7 @@
         <v>554</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="296" spans="1:3">
@@ -5701,7 +5699,7 @@
         <v>555</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="297" spans="1:3">
@@ -5712,12 +5710,12 @@
         <v>600</v>
       </c>
       <c r="C297" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="298" spans="1:3">
       <c r="A298" s="6" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B298" s="3">
         <v>601</v>
@@ -5734,12 +5732,12 @@
         <v>602</v>
       </c>
       <c r="C299" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="300" spans="1:3">
       <c r="A300" s="6" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B300" s="3">
         <v>603</v>
@@ -5756,7 +5754,7 @@
         <v>604</v>
       </c>
       <c r="C301" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="302" spans="1:3">
@@ -5767,7 +5765,7 @@
         <v>605</v>
       </c>
       <c r="C302" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="303" spans="1:3">
@@ -5778,7 +5776,7 @@
         <v>606</v>
       </c>
       <c r="C303" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="304" spans="1:3">
@@ -5789,12 +5787,12 @@
         <v>607</v>
       </c>
       <c r="C304" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="305" spans="1:3">
       <c r="A305" s="6" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B305" s="3">
         <v>608</v>
@@ -5838,7 +5836,7 @@
     </row>
     <row r="309" spans="1:3">
       <c r="A309" s="6" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B309" s="3">
         <v>612</v>
@@ -5855,7 +5853,7 @@
         <v>613</v>
       </c>
       <c r="C310" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="311" spans="1:3">
@@ -5882,7 +5880,7 @@
     </row>
     <row r="313" spans="1:3">
       <c r="A313" s="6" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="B313" s="3">
         <v>616</v>
@@ -5893,7 +5891,7 @@
     </row>
     <row r="314" spans="1:3">
       <c r="A314" s="6" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B314" s="3">
         <v>617</v>
@@ -5904,7 +5902,7 @@
     </row>
     <row r="315" spans="1:3">
       <c r="A315" s="6" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="B315" s="3">
         <v>618</v>
@@ -5948,7 +5946,7 @@
     </row>
     <row r="319" spans="1:3">
       <c r="A319" s="6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B319" s="3">
         <v>622</v>
@@ -5959,7 +5957,7 @@
     </row>
     <row r="320" spans="1:3">
       <c r="A320" s="6" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B320" s="3">
         <v>623</v>
@@ -5970,7 +5968,7 @@
     </row>
     <row r="321" spans="1:3">
       <c r="A321" s="6" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="B321" s="3">
         <v>624</v>
@@ -5981,7 +5979,7 @@
     </row>
     <row r="322" spans="1:3">
       <c r="A322" s="6" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B322" s="3">
         <v>625</v>
@@ -5992,7 +5990,7 @@
     </row>
     <row r="323" spans="1:3">
       <c r="A323" s="6" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B323" s="3">
         <v>626</v>
@@ -6014,13 +6012,13 @@
     </row>
     <row r="325" spans="1:3">
       <c r="A325" s="6" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="B325" s="3">
         <v>628</v>
       </c>
       <c r="C325" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="326" spans="1:3">
@@ -6031,7 +6029,7 @@
         <v>629</v>
       </c>
       <c r="C326" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="327" spans="1:3">
@@ -6064,12 +6062,12 @@
         <v>632</v>
       </c>
       <c r="C329" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="330" spans="1:3">
       <c r="A330" s="6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B330" s="3">
         <v>633</v>
@@ -6080,7 +6078,7 @@
     </row>
     <row r="331" spans="1:3">
       <c r="A331" s="6" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B331" s="3">
         <v>634</v>
@@ -6091,7 +6089,7 @@
     </row>
     <row r="332" spans="1:3">
       <c r="A332" s="6" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="B332" s="3">
         <v>635</v>
@@ -6108,7 +6106,7 @@
         <v>636</v>
       </c>
       <c r="C333" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="334" spans="1:3">
@@ -6124,13 +6122,13 @@
     </row>
     <row r="335" spans="1:3">
       <c r="A335" s="6" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="B335" s="3">
         <v>638</v>
       </c>
       <c r="C335" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="336" spans="1:3">
@@ -6146,7 +6144,7 @@
     </row>
     <row r="337" spans="1:3">
       <c r="A337" s="6" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B337" s="3">
         <v>701</v>
@@ -6179,7 +6177,7 @@
     </row>
     <row r="340" spans="1:3">
       <c r="A340" s="6" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B340" s="3">
         <v>704</v>
@@ -6190,7 +6188,7 @@
     </row>
     <row r="341" spans="1:3">
       <c r="A341" s="6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B341" s="3">
         <v>705</v>
@@ -6223,7 +6221,7 @@
     </row>
     <row r="344" spans="1:3">
       <c r="A344" s="6" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="B344" s="3">
         <v>708</v>
@@ -6251,12 +6249,12 @@
         <v>710</v>
       </c>
       <c r="C346" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="347" spans="1:3">
       <c r="A347" s="6" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="B347" s="3">
         <v>711</v>
@@ -6273,7 +6271,7 @@
         <v>712</v>
       </c>
       <c r="C348" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="349" spans="1:3">
@@ -6284,7 +6282,7 @@
         <v>713</v>
       </c>
       <c r="C349" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="350" spans="1:3">
@@ -6311,7 +6309,7 @@
     </row>
     <row r="352" spans="1:3">
       <c r="A352" s="6" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="B352" s="3">
         <v>716</v>
@@ -6333,7 +6331,7 @@
     </row>
     <row r="354" spans="1:3">
       <c r="A354" s="6" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B354" s="3">
         <v>718</v>
@@ -6366,7 +6364,7 @@
     </row>
     <row r="357" spans="1:3">
       <c r="A357" s="6" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="B357" s="3">
         <v>721</v>
@@ -6388,7 +6386,7 @@
     </row>
     <row r="359" spans="1:3">
       <c r="A359" s="6" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="B359" s="3">
         <v>723</v>
@@ -6410,7 +6408,7 @@
     </row>
     <row r="361" spans="1:3">
       <c r="A361" s="6" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B361" s="3">
         <v>725</v>
@@ -6421,7 +6419,7 @@
     </row>
     <row r="362" spans="1:3">
       <c r="A362" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B362" s="3">
         <v>726</v>
@@ -6432,7 +6430,7 @@
     </row>
     <row r="363" spans="1:3">
       <c r="A363" s="6" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B363" s="3">
         <v>727</v>
@@ -6515,12 +6513,12 @@
         <v>734</v>
       </c>
       <c r="C370" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="371" spans="1:3">
       <c r="A371" s="6" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B371" s="3">
         <v>735</v>
@@ -6537,12 +6535,12 @@
         <v>736</v>
       </c>
       <c r="C372" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="373" spans="1:3">
       <c r="A373" s="6" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B373" s="3">
         <v>737</v>
@@ -6586,7 +6584,7 @@
     </row>
     <row r="377" spans="1:3">
       <c r="A377" s="6" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B377" s="3">
         <v>741</v>
@@ -6702,7 +6700,7 @@
         <v>751</v>
       </c>
       <c r="C387" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="388" spans="1:3">
@@ -6713,7 +6711,7 @@
         <v>752</v>
       </c>
       <c r="C388" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="389" spans="1:3">
@@ -6729,7 +6727,7 @@
     </row>
     <row r="390" spans="1:3">
       <c r="A390" s="6" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="B390" s="3">
         <v>801</v>
@@ -6762,7 +6760,7 @@
     </row>
     <row r="393" spans="1:3">
       <c r="A393" s="6" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B393" s="3">
         <v>804</v>
@@ -6773,7 +6771,7 @@
     </row>
     <row r="394" spans="1:3">
       <c r="A394" s="6" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="B394" s="3">
         <v>805</v>
@@ -6795,7 +6793,7 @@
     </row>
     <row r="396" spans="1:3">
       <c r="A396" s="6" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="B396" s="3">
         <v>807</v>
@@ -6828,7 +6826,7 @@
     </row>
     <row r="399" spans="1:3">
       <c r="A399" s="6" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="B399" s="3">
         <v>810</v>
@@ -6845,7 +6843,7 @@
         <v>811</v>
       </c>
       <c r="C400" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="401" spans="1:3">
@@ -6872,7 +6870,7 @@
     </row>
     <row r="403" spans="1:3">
       <c r="A403" s="6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B403" s="3">
         <v>814</v>
@@ -6900,12 +6898,12 @@
         <v>816</v>
       </c>
       <c r="C405" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="406" spans="1:3">
       <c r="A406" s="6" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="B406" s="3">
         <v>817</v>
@@ -6927,7 +6925,7 @@
     </row>
     <row r="408" spans="1:3">
       <c r="A408" s="6" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B408" s="3">
         <v>901</v>
@@ -6960,7 +6958,7 @@
     </row>
     <row r="411" spans="1:3">
       <c r="A411" s="6" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="B411" s="3">
         <v>904</v>
@@ -7048,7 +7046,7 @@
     </row>
     <row r="419" spans="1:3">
       <c r="A419" s="6" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B419" s="3">
         <v>912</v>
@@ -7070,7 +7068,7 @@
     </row>
     <row r="421" spans="1:3">
       <c r="A421" s="6" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="B421" s="3">
         <v>914</v>
@@ -7092,7 +7090,7 @@
     </row>
     <row r="423" spans="1:3">
       <c r="A423" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B423" s="3">
         <v>916</v>
@@ -7125,7 +7123,7 @@
     </row>
     <row r="426" spans="1:3">
       <c r="A426" s="6" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B426" s="3">
         <v>919</v>
@@ -7142,12 +7140,12 @@
         <v>920</v>
       </c>
       <c r="C427" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="428" spans="1:3">
       <c r="A428" s="6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B428" s="3">
         <v>921</v>
@@ -7158,7 +7156,7 @@
     </row>
     <row r="429" spans="1:3">
       <c r="A429" s="6" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B429" s="3">
         <v>922</v>
@@ -7180,7 +7178,7 @@
     </row>
     <row r="431" spans="1:3">
       <c r="A431" s="6" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="B431" s="3">
         <v>924</v>
@@ -7202,7 +7200,7 @@
     </row>
     <row r="433" spans="1:3">
       <c r="A433" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="B433" s="3">
         <v>926</v>
@@ -7230,12 +7228,12 @@
         <v>928</v>
       </c>
       <c r="C435" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="436" spans="1:3">
       <c r="A436" s="6" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B436" s="3">
         <v>929</v>
@@ -7252,7 +7250,7 @@
         <v>930</v>
       </c>
       <c r="C437" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="438" spans="1:3">
@@ -7263,18 +7261,18 @@
         <v>931</v>
       </c>
       <c r="C438" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="439" spans="1:3">
       <c r="A439" s="6" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="B439" s="3">
         <v>932</v>
       </c>
       <c r="C439" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="440" spans="1:3">
@@ -7285,7 +7283,7 @@
         <v>933</v>
       </c>
       <c r="C440" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="441" spans="1:3">
@@ -7296,7 +7294,7 @@
         <v>934</v>
       </c>
       <c r="C441" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="442" spans="1:3">
@@ -7307,7 +7305,7 @@
         <v>935</v>
       </c>
       <c r="C442" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="443" spans="1:3">
@@ -7318,7 +7316,7 @@
         <v>936</v>
       </c>
       <c r="C443" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="444" spans="1:3">
@@ -7329,7 +7327,7 @@
         <v>937</v>
       </c>
       <c r="C444" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="445" spans="1:3">
@@ -7466,7 +7464,7 @@
     </row>
     <row r="457" spans="1:3">
       <c r="A457" s="6" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B457" s="3">
         <v>1012</v>
@@ -7498,14 +7496,14 @@
       </c>
     </row>
     <row r="460" spans="1:3">
-      <c r="A460" s="6" t="s">
-        <v>616</v>
+      <c r="A460" s="6">
+        <v>10</v>
       </c>
       <c r="B460" s="3">
         <v>1015</v>
       </c>
       <c r="C460" t="s">
-        <v>546</v>
+        <v>618</v>
       </c>
     </row>
     <row r="461" spans="1:3">
@@ -7532,7 +7530,7 @@
     </row>
     <row r="463" spans="1:3">
       <c r="A463" s="6" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B463" s="3">
         <v>1018</v>
@@ -7554,7 +7552,7 @@
     </row>
     <row r="465" spans="1:3">
       <c r="A465" s="6" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B465" s="3">
         <v>1020</v>
@@ -7576,7 +7574,7 @@
     </row>
     <row r="467" spans="1:3">
       <c r="A467" s="6" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="B467" s="3">
         <v>1022</v>
@@ -7587,7 +7585,7 @@
     </row>
     <row r="468" spans="1:3">
       <c r="A468" s="6" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B468" s="3">
         <v>1023</v>
@@ -7598,7 +7596,7 @@
     </row>
     <row r="469" spans="1:3">
       <c r="A469" s="6" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B469" s="3">
         <v>1024</v>
@@ -7609,7 +7607,7 @@
     </row>
     <row r="470" spans="1:3">
       <c r="A470" s="6" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B470" s="3">
         <v>1025</v>
@@ -7642,7 +7640,7 @@
     </row>
     <row r="473" spans="1:3">
       <c r="A473" s="6" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B473" s="3">
         <v>1028</v>
@@ -7664,7 +7662,7 @@
     </row>
     <row r="475" spans="1:3">
       <c r="A475" s="6" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B475" s="3">
         <v>1030</v>
@@ -7675,7 +7673,7 @@
     </row>
     <row r="476" spans="1:3">
       <c r="A476" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B476" s="3">
         <v>1031</v>
@@ -7686,7 +7684,7 @@
     </row>
     <row r="477" spans="1:3">
       <c r="A477" s="6" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B477" s="3">
         <v>1032</v>
@@ -7697,7 +7695,7 @@
     </row>
     <row r="478" spans="1:3">
       <c r="A478" s="6" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="B478" s="3">
         <v>1033</v>
@@ -7708,7 +7706,7 @@
     </row>
     <row r="479" spans="1:3">
       <c r="A479" s="6" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="B479" s="3">
         <v>1034</v>
@@ -7719,7 +7717,7 @@
     </row>
     <row r="480" spans="1:3">
       <c r="A480" s="6" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="B480" s="3">
         <v>1035</v>
@@ -7873,7 +7871,7 @@
     </row>
     <row r="494" spans="1:3">
       <c r="A494" s="6" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="B494" s="3">
         <v>1049</v>
@@ -7890,7 +7888,7 @@
         <v>1050</v>
       </c>
       <c r="C495" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="496" spans="1:3">
@@ -7912,7 +7910,7 @@
         <v>1052</v>
       </c>
       <c r="C497" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="498" spans="1:3">
@@ -7928,7 +7926,7 @@
     </row>
     <row r="499" spans="1:3">
       <c r="A499" s="6" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B499" s="3">
         <v>1054</v>
@@ -7939,7 +7937,7 @@
     </row>
     <row r="500" spans="1:3">
       <c r="A500" s="6" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B500" s="3">
         <v>1100</v>
@@ -7950,18 +7948,18 @@
     </row>
     <row r="501" spans="1:3">
       <c r="A501" s="6" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="B501" s="3">
         <v>1101</v>
       </c>
       <c r="C501" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="502" spans="1:3">
       <c r="A502" s="6" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B502" s="3">
         <v>1102</v>
@@ -7972,7 +7970,7 @@
     </row>
     <row r="503" spans="1:3">
       <c r="A503" s="6" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B503" s="3">
         <v>1103</v>
@@ -7983,18 +7981,18 @@
     </row>
     <row r="504" spans="1:3">
       <c r="A504" s="6" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="B504" s="3">
         <v>1104</v>
       </c>
       <c r="C504" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="505" spans="1:3">
       <c r="A505" s="6" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B505" s="3">
         <v>1105</v>
@@ -8033,7 +8031,7 @@
         <v>1108</v>
       </c>
       <c r="C508" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="509" spans="1:3">
@@ -8044,7 +8042,7 @@
         <v>1109</v>
       </c>
       <c r="C509" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="510" spans="1:3">
@@ -8071,13 +8069,13 @@
     </row>
     <row r="512" spans="1:3">
       <c r="A512" s="6" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="B512" s="3">
         <v>1112</v>
       </c>
       <c r="C512" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="513" spans="1:3">
@@ -8088,56 +8086,56 @@
         <v>1113</v>
       </c>
       <c r="C513" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="514" spans="1:3">
       <c r="A514" s="6" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B514" s="3">
         <v>1200</v>
       </c>
       <c r="C514" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="515" spans="1:3">
       <c r="A515" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B515" s="3">
         <v>1201</v>
       </c>
       <c r="C515" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="516" spans="1:3">
       <c r="A516" s="6" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B516" s="3">
         <v>1202</v>
       </c>
       <c r="C516" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="517" spans="1:3">
       <c r="A517" s="6" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="B517" s="3">
         <v>1203</v>
       </c>
       <c r="C517" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="518" spans="1:3">
       <c r="A518" s="6" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="B518" s="3">
         <v>1204</v>
@@ -8148,7 +8146,7 @@
     </row>
     <row r="519" spans="1:3">
       <c r="A519" s="6" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="B519" s="3">
         <v>1205</v>
@@ -8159,7 +8157,7 @@
     </row>
     <row r="520" spans="1:3">
       <c r="A520" s="6" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="B520" s="3">
         <v>1206</v>
@@ -8368,18 +8366,18 @@
     </row>
     <row r="539" spans="1:3">
       <c r="A539" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B539" s="4">
         <v>1300</v>
       </c>
       <c r="C539" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="540" spans="1:3">
       <c r="A540" s="6" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B540" s="3">
         <v>1301</v>
@@ -8412,7 +8410,7 @@
     </row>
     <row r="543" spans="1:3">
       <c r="A543" s="6" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="B543" s="3">
         <v>1304</v>
@@ -8423,7 +8421,7 @@
     </row>
     <row r="544" spans="1:3">
       <c r="A544" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="B544" s="3">
         <v>1305</v>
@@ -8434,7 +8432,7 @@
     </row>
     <row r="545" spans="1:3">
       <c r="A545" s="6" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B545" s="4">
         <v>1306</v>
@@ -8456,7 +8454,7 @@
     </row>
     <row r="547" spans="1:3">
       <c r="A547" s="6" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B547" s="3">
         <v>1308</v>
@@ -8473,7 +8471,7 @@
         <v>1309</v>
       </c>
       <c r="C548" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="549" spans="1:3">
@@ -8495,12 +8493,12 @@
         <v>1311</v>
       </c>
       <c r="C550" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="551" spans="1:3">
       <c r="A551" s="6" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B551" s="4">
         <v>1312</v>
@@ -8511,7 +8509,7 @@
     </row>
     <row r="552" spans="1:3">
       <c r="A552" s="6" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="B552" s="3">
         <v>1313</v>
@@ -8544,7 +8542,7 @@
     </row>
     <row r="555" spans="1:3">
       <c r="A555" s="6" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="B555" s="3">
         <v>1316</v>
@@ -8599,7 +8597,7 @@
     </row>
     <row r="560" spans="1:3">
       <c r="A560" s="6" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B560" s="4">
         <v>1321</v>
@@ -8610,7 +8608,7 @@
     </row>
     <row r="561" spans="1:3">
       <c r="A561" s="6" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B561" s="3">
         <v>1322</v>
@@ -8660,7 +8658,7 @@
         <v>1326</v>
       </c>
       <c r="C565" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="566" spans="1:3">
@@ -8671,18 +8669,18 @@
         <v>1327</v>
       </c>
       <c r="C566" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="567" spans="1:3">
-      <c r="A567" s="6" t="s">
-        <v>616</v>
+      <c r="A567" s="6">
+        <v>13</v>
       </c>
       <c r="B567" s="3">
         <v>1328</v>
       </c>
       <c r="C567" t="s">
-        <v>411</v>
+        <v>543</v>
       </c>
     </row>
     <row r="568" spans="1:3">
@@ -8764,7 +8762,7 @@
     </row>
     <row r="575" spans="1:3">
       <c r="A575" s="6" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B575" s="4">
         <v>1336</v>
@@ -8781,7 +8779,7 @@
         <v>1337</v>
       </c>
       <c r="C576" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="577" spans="1:3">
@@ -8792,7 +8790,7 @@
         <v>1338</v>
       </c>
       <c r="C577" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="578" spans="1:3">
@@ -8803,7 +8801,7 @@
         <v>1339</v>
       </c>
       <c r="C578" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="579" spans="1:3">
@@ -8814,7 +8812,7 @@
         <v>1340</v>
       </c>
       <c r="C579" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="580" spans="1:3">
@@ -8825,89 +8823,89 @@
         <v>1341</v>
       </c>
       <c r="C580" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="581" spans="1:3">
       <c r="A581" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B581" s="4">
         <v>1342</v>
       </c>
       <c r="C581" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="582" spans="1:3">
       <c r="A582" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B582" s="3">
         <v>1343</v>
       </c>
       <c r="C582" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="583" spans="1:3">
       <c r="A583" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B583" s="3">
         <v>1344</v>
       </c>
       <c r="C583" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="584" spans="1:3">
       <c r="A584" s="6" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B584" s="4">
         <v>1345</v>
       </c>
       <c r="C584" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="585" spans="1:3">
       <c r="A585" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B585" s="3">
         <v>1346</v>
       </c>
       <c r="C585" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="586" spans="1:3">
       <c r="A586" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B586" s="3">
         <v>1347</v>
       </c>
       <c r="C586" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="587" spans="1:3">
       <c r="A587" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B587" s="4">
         <v>1348</v>
       </c>
       <c r="C587" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="588" spans="1:3">
       <c r="A588" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B588" s="3">
         <v>1349</v>
@@ -8946,7 +8944,7 @@
         <v>1352</v>
       </c>
       <c r="C591" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="592" spans="1:3">
@@ -8990,7 +8988,7 @@
         <v>1356</v>
       </c>
       <c r="C595" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="596" spans="1:3">
@@ -9023,7 +9021,7 @@
         <v>1359</v>
       </c>
       <c r="C598" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="599" spans="1:3">
@@ -9034,7 +9032,7 @@
         <v>1360</v>
       </c>
       <c r="C599" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="600" spans="1:3">
@@ -9045,56 +9043,56 @@
         <v>1361</v>
       </c>
       <c r="C600" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="601" spans="1:3">
       <c r="A601" s="6" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B601" s="3">
         <v>1362</v>
       </c>
       <c r="C601" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="602" spans="1:3">
       <c r="A602" s="6" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B602" s="3">
         <v>1400</v>
       </c>
       <c r="C602" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="603" spans="1:3">
       <c r="A603" s="6" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="B603" s="3">
         <v>1401</v>
       </c>
       <c r="C603" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="604" spans="1:3">
       <c r="A604" s="6" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="B604" s="3">
         <v>1402</v>
       </c>
       <c r="C604" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="605" spans="1:3">
       <c r="A605" s="6" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B605" s="3">
         <v>1403</v>
@@ -9105,13 +9103,13 @@
     </row>
     <row r="606" spans="1:3">
       <c r="A606" s="6" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B606" s="3">
         <v>1404</v>
       </c>
       <c r="C606" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="607" spans="1:3">
@@ -9122,7 +9120,7 @@
         <v>1405</v>
       </c>
       <c r="C607" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="608" spans="1:3">
@@ -9133,7 +9131,7 @@
         <v>1406</v>
       </c>
       <c r="C608" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="609" spans="1:3">
@@ -9144,29 +9142,29 @@
         <v>1407</v>
       </c>
       <c r="C609" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="610" spans="1:3">
       <c r="A610" s="6" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B610" s="3">
         <v>1408</v>
       </c>
       <c r="C610" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="611" spans="1:3">
       <c r="A611" s="6" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B611" s="3">
         <v>1409</v>
       </c>
       <c r="C611" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="612" spans="1:3">
@@ -9177,7 +9175,7 @@
         <v>1410</v>
       </c>
       <c r="C612" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="613" spans="1:3">
@@ -9188,7 +9186,7 @@
         <v>1411</v>
       </c>
       <c r="C613" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="614" spans="1:3">
@@ -9199,7 +9197,7 @@
         <v>1412</v>
       </c>
       <c r="C614" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="615" spans="1:3">
@@ -9210,7 +9208,7 @@
         <v>1413</v>
       </c>
       <c r="C615" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="616" spans="1:3">
@@ -9221,7 +9219,7 @@
         <v>1414</v>
       </c>
       <c r="C616" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="617" spans="1:3">
@@ -9232,18 +9230,18 @@
         <v>1415</v>
       </c>
       <c r="C617" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="618" spans="1:3">
       <c r="A618" s="6" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="B618" s="4">
         <v>1500</v>
       </c>
       <c r="C618" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="619" spans="1:3">
@@ -9254,7 +9252,7 @@
         <v>1501</v>
       </c>
       <c r="C619" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="620" spans="1:3">
@@ -9265,7 +9263,7 @@
         <v>1502</v>
       </c>
       <c r="C620" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="621" spans="1:3">
@@ -9276,7 +9274,7 @@
         <v>1503</v>
       </c>
       <c r="C621" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="622" spans="1:3">
@@ -9287,7 +9285,7 @@
         <v>1504</v>
       </c>
       <c r="C622" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="623" spans="1:3">
@@ -9298,12 +9296,12 @@
         <v>1505</v>
       </c>
       <c r="C623" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="624" spans="1:3">
       <c r="A624" s="6" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B624" s="4">
         <v>1600</v>
@@ -9314,24 +9312,24 @@
     </row>
     <row r="625" spans="1:3">
       <c r="A625" s="6" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="B625" s="4">
         <v>1601</v>
       </c>
       <c r="C625" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="626" spans="1:3">
       <c r="A626" s="6" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="B626" s="4">
         <v>1602</v>
       </c>
       <c r="C626" s="2" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="627" spans="1:3">
@@ -9342,7 +9340,7 @@
         <v>1603</v>
       </c>
       <c r="C627" s="2" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="628" spans="1:3">
@@ -9353,7 +9351,7 @@
         <v>1604</v>
       </c>
       <c r="C628" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="629" spans="1:3">
@@ -9364,7 +9362,7 @@
         <v>1605</v>
       </c>
       <c r="C629" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="630" spans="1:3">
@@ -9375,7 +9373,7 @@
         <v>1606</v>
       </c>
       <c r="C630" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="631" spans="1:3">
@@ -9386,7 +9384,7 @@
         <v>1607</v>
       </c>
       <c r="C631" s="2" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="632" spans="1:3">
@@ -9397,7 +9395,7 @@
         <v>1608</v>
       </c>
       <c r="C632" s="2" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="633" spans="1:3">
@@ -9408,7 +9406,7 @@
         <v>1609</v>
       </c>
       <c r="C633" s="2" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="634" spans="1:3">
@@ -9419,7 +9417,7 @@
         <v>1610</v>
       </c>
       <c r="C634" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="635" spans="1:3">
@@ -9430,7 +9428,7 @@
         <v>1611</v>
       </c>
       <c r="C635" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="636" spans="1:3">
@@ -9441,7 +9439,7 @@
         <v>1612</v>
       </c>
       <c r="C636" s="2" t="s">
-        <v>519</v>
+        <v>616</v>
       </c>
     </row>
   </sheetData>

</xml_diff>